<commit_message>
Fix iOS bundle identifier to com.yaosulee.bonegood
</commit_message>
<xml_diff>
--- a/紀錄.xlsx
+++ b/紀錄.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\202510Mobile\yaosuleemobile_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADBBBE7-55DA-4622-9E76-6FB79F8FD480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE22AED-ADF1-40A4-8F4C-2C8939A86C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11610" yWindow="30" windowWidth="15330" windowHeight="14805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7995" yWindow="1290" windowWidth="22470" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="儲存 key.jks" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>輸入金鑰庫密碼</t>
   </si>
@@ -173,6 +173,13 @@
   </si>
   <si>
     <t>android:label="YaosuLee"</t>
+  </si>
+  <si>
+    <t>pubspec.yaml</t>
+  </si>
+  <si>
+    <t>版次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -515,7 +522,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -608,10 +615,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F916F7C-3E6A-4CF9-A8BF-DCD8C0B15BC4}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -668,6 +675,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:12">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -679,11 +694,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DB3413-0C04-4CA8-8DCE-E50FBC1ECA75}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>